<commit_message>
Re-run Q07–Q09 after stricter Coding threshold in Q06 (≥5 prompts & cos≥0.45)
</commit_message>
<xml_diff>
--- a/results/answers_q06.xlsx
+++ b/results/answers_q06.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Writing &amp; professional communication|Brainstorming &amp; personal ideas - fun|Coding - programming help|Language practice or translation|Study revision - exam prep|Other</t>
+          <t>Writing &amp; professional communication|Coding - programming help|Study revision - exam prep|Other</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -476,7 +476,7 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45841.54698783338</v>
+        <v>45841.64214048738</v>
       </c>
     </row>
     <row r="3">
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45841.54698783338</v>
+        <v>45841.64214048738</v>
       </c>
     </row>
     <row r="4">
@@ -507,7 +507,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Brainstorming &amp; personal ideas - fun|Coding - programming help|Other</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45841.54698783338</v>
+        <v>45841.64214048738</v>
       </c>
     </row>
     <row r="5">
@@ -527,7 +527,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Writing &amp; professional communication|Coding - programming help|Study revision - exam prep|Other</t>
+          <t>Writing &amp; professional communication|Coding - programming help|Other</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45841.54698783338</v>
+        <v>45841.64214048738</v>
       </c>
     </row>
     <row r="6">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>45841.54698783338</v>
+        <v>45841.64214048738</v>
       </c>
     </row>
     <row r="7">
@@ -567,7 +567,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Writing &amp; professional communication|Brainstorming &amp; personal ideas - fun|Coding - programming help|Language practice or translation|Study revision - exam prep|Other</t>
+          <t>Writing &amp; professional communication|Brainstorming &amp; personal ideas - fun|Language practice or translation|Other</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -576,7 +576,7 @@
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>45841.54698783338</v>
+        <v>45841.64214048738</v>
       </c>
     </row>
     <row r="8">
@@ -587,7 +587,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Writing &amp; professional communication|Coding - programming help|Study revision - exam prep|Other</t>
+          <t>Writing &amp; professional communication|Coding - programming help|Other</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>45841.54698783338</v>
+        <v>45841.64214048738</v>
       </c>
     </row>
     <row r="9">
@@ -607,7 +607,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Writing &amp; professional communication|Brainstorming &amp; personal ideas - fun|Coding - programming help|Language practice or translation|Study revision - exam prep|Other</t>
+          <t>Writing &amp; professional communication|Brainstorming &amp; personal ideas - fun|Coding - programming help|Language practice or translation|Other</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>45841.54698783338</v>
+        <v>45841.64214048738</v>
       </c>
     </row>
   </sheetData>

</xml_diff>